<commit_message>
Impl our case with VRP program multi vehicle
</commit_message>
<xml_diff>
--- a/Azores_Flight_Data_v4.xlsx
+++ b/Azores_Flight_Data_v4.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nils de Krom\Documents\GitHub\Operations_optimization_assignment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5A7AE42-5732-4319-A43D-52D2C6254B87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{414179CD-7887-496E-AA7E-A1FA3073F908}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="19090" yWindow="-110" windowWidth="25820" windowHeight="14020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Demand Table" sheetId="4" r:id="rId1"/>
@@ -938,8 +938,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:S1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.59765625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1037,32 +1037,32 @@
         <v>9307.8750664956679</v>
       </c>
       <c r="E3" s="28">
-        <v>10</v>
+        <v>37</v>
       </c>
       <c r="F3" s="28">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="G3" s="28">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="H3" s="28">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="I3" s="28">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="J3" s="28">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="K3" s="28">
-        <v>10</v>
+        <v>60</v>
       </c>
       <c r="L3" s="28">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="M3" s="17">
         <f>SUM(D3:L3)</f>
-        <v>9387.8750664956679</v>
+        <v>9524.8750664956679</v>
       </c>
     </row>
     <row r="4" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1197,7 +1197,7 @@
         <v>12</v>
       </c>
       <c r="D11" s="30">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="F11" s="20"/>
       <c r="G11" s="20"/>
@@ -1222,7 +1222,7 @@
         <v>13</v>
       </c>
       <c r="D12" s="30">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="F12" s="20"/>
       <c r="G12" s="20"/>
@@ -1247,7 +1247,7 @@
         <v>14</v>
       </c>
       <c r="D13" s="30">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="F13" s="17"/>
       <c r="G13" s="17"/>
@@ -1272,7 +1272,7 @@
         <v>15</v>
       </c>
       <c r="D14" s="30">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="O14" s="53"/>
       <c r="P14" s="50"/>
@@ -1288,7 +1288,7 @@
         <v>16</v>
       </c>
       <c r="D15" s="30">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="O15" s="53"/>
       <c r="P15" s="51"/>
@@ -1304,7 +1304,7 @@
         <v>17</v>
       </c>
       <c r="D16" s="30">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="O16" s="53"/>
       <c r="P16" s="50"/>
@@ -1320,7 +1320,7 @@
         <v>18</v>
       </c>
       <c r="D17" s="30">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="O17" s="49"/>
       <c r="P17" s="50"/>
@@ -1335,7 +1335,7 @@
         <v>20</v>
       </c>
       <c r="D18" s="30">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="O18" s="50"/>
       <c r="P18" s="50"/>
@@ -1349,7 +1349,7 @@
       <c r="C19" s="72"/>
       <c r="D19" s="17">
         <f>SUM(D10:D18)</f>
-        <v>9387.8750664956679</v>
+        <v>9467.8750664956679</v>
       </c>
       <c r="O19" s="50"/>
       <c r="P19" s="54"/>
@@ -3931,7 +3931,7 @@
         <v>43.358360000000005</v>
       </c>
       <c r="G4" s="64">
-        <f t="shared" ref="G2:G12" si="4">B4*$B$31</f>
+        <f t="shared" ref="G4:G12" si="4">B4*$B$31</f>
         <v>728.6400000000001</v>
       </c>
       <c r="H4" s="64">
@@ -4312,7 +4312,7 @@
   </sheetPr>
   <dimension ref="A1:M12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
added class for final azor program
</commit_message>
<xml_diff>
--- a/Azores_Flight_Data_v4.xlsx
+++ b/Azores_Flight_Data_v4.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nils de Krom\Documents\GitHub\Operations_optimization_assignment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{242C2396-3D9A-42BD-A578-CD7BA1ECC389}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1262491-1440-4A01-81AE-D55E08F88EA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19090" yWindow="-110" windowWidth="25820" windowHeight="14020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Demand Table" sheetId="4" r:id="rId1"/>
@@ -736,14 +736,14 @@
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="2" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="2" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -962,7 +962,7 @@
   <dimension ref="A1:S1000"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.59765625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1009,7 +1009,7 @@
       <c r="L1" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="M1" s="71" t="s">
+      <c r="M1" s="75" t="s">
         <v>11</v>
       </c>
     </row>
@@ -1044,7 +1044,7 @@
       <c r="L2" s="25" t="s">
         <v>20</v>
       </c>
-      <c r="M2" s="72"/>
+      <c r="M2" s="76"/>
     </row>
     <row r="3" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="26" t="s">
@@ -1062,25 +1062,25 @@
       <c r="E3" s="28">
         <v>32</v>
       </c>
-      <c r="F3" s="73">
+      <c r="F3" s="71">
         <v>6</v>
       </c>
-      <c r="G3" s="73">
+      <c r="G3" s="71">
         <v>22</v>
       </c>
-      <c r="H3" s="73">
+      <c r="H3" s="71">
         <v>45</v>
       </c>
-      <c r="I3" s="73">
+      <c r="I3" s="71">
         <v>0</v>
       </c>
-      <c r="J3" s="73">
+      <c r="J3" s="71">
         <v>44</v>
       </c>
-      <c r="K3" s="73">
+      <c r="K3" s="71">
         <v>51</v>
       </c>
-      <c r="L3" s="73">
+      <c r="L3" s="71">
         <v>61</v>
       </c>
       <c r="M3" s="17">
@@ -1089,31 +1089,31 @@
       </c>
     </row>
     <row r="4" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D4" s="73">
+      <c r="D4" s="71">
         <v>9308</v>
       </c>
-      <c r="E4" s="73">
+      <c r="E4" s="71">
         <v>32</v>
       </c>
-      <c r="F4" s="73">
+      <c r="F4" s="71">
         <v>246</v>
       </c>
-      <c r="G4" s="73">
+      <c r="G4" s="71">
         <v>982</v>
       </c>
-      <c r="H4" s="73">
+      <c r="H4" s="71">
         <v>925</v>
       </c>
-      <c r="I4" s="73">
+      <c r="I4" s="71">
         <v>560</v>
       </c>
-      <c r="J4" s="73">
+      <c r="J4" s="71">
         <v>284</v>
       </c>
-      <c r="K4" s="73">
+      <c r="K4" s="71">
         <v>3731</v>
       </c>
-      <c r="L4" s="73">
+      <c r="L4" s="71">
         <v>381</v>
       </c>
       <c r="O4" s="50"/>
@@ -1121,85 +1121,85 @@
       <c r="Q4" s="50"/>
     </row>
     <row r="5" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D5" s="73"/>
-      <c r="E5" s="73">
+      <c r="D5" s="71"/>
+      <c r="E5" s="71">
         <f>E4/80</f>
         <v>0.4</v>
       </c>
-      <c r="F5" s="73">
+      <c r="F5" s="71">
         <f t="shared" ref="F5:L5" si="0">F4/80</f>
         <v>3.0750000000000002</v>
       </c>
-      <c r="G5" s="73">
+      <c r="G5" s="71">
         <f t="shared" si="0"/>
         <v>12.275</v>
       </c>
-      <c r="H5" s="73">
+      <c r="H5" s="71">
         <f t="shared" si="0"/>
         <v>11.5625</v>
       </c>
-      <c r="I5" s="73">
+      <c r="I5" s="71">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="J5" s="73">
+      <c r="J5" s="71">
         <f t="shared" si="0"/>
         <v>3.55</v>
       </c>
-      <c r="K5" s="73">
+      <c r="K5" s="71">
         <f t="shared" si="0"/>
         <v>46.637500000000003</v>
       </c>
-      <c r="L5" s="73">
+      <c r="L5" s="71">
         <f t="shared" si="0"/>
         <v>4.7625000000000002</v>
       </c>
-      <c r="M5" s="74"/>
+      <c r="M5" s="72"/>
       <c r="N5" s="17"/>
       <c r="O5" s="50"/>
       <c r="P5" s="50"/>
       <c r="Q5" s="50"/>
     </row>
     <row r="6" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D6" s="73"/>
-      <c r="E6" s="74">
+      <c r="D6" s="71"/>
+      <c r="E6" s="72">
         <f>ROUNDDOWN(E5,0)</f>
         <v>0</v>
       </c>
-      <c r="F6" s="74">
+      <c r="F6" s="72">
         <f>ROUNDDOWN(F5,0)</f>
         <v>3</v>
       </c>
-      <c r="G6" s="74">
+      <c r="G6" s="72">
         <f t="shared" ref="G6:L6" si="1">ROUNDDOWN(G5,0)</f>
         <v>12</v>
       </c>
-      <c r="H6" s="74">
+      <c r="H6" s="72">
         <f t="shared" si="1"/>
         <v>11</v>
       </c>
-      <c r="I6" s="74">
+      <c r="I6" s="72">
         <f t="shared" si="1"/>
         <v>7</v>
       </c>
-      <c r="J6" s="74">
+      <c r="J6" s="72">
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
-      <c r="K6" s="74">
+      <c r="K6" s="72">
         <f t="shared" si="1"/>
         <v>46</v>
       </c>
-      <c r="L6" s="74">
+      <c r="L6" s="72">
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="M6" s="74"/>
-      <c r="N6" s="76">
+      <c r="M6" s="72"/>
+      <c r="N6" s="74">
         <f>SUM(E6:L6) * 2</f>
         <v>172</v>
       </c>
-      <c r="O6" s="75" t="s">
+      <c r="O6" s="73" t="s">
         <v>71</v>
       </c>
       <c r="P6" s="50"/>
@@ -1245,7 +1245,7 @@
         <v>61</v>
       </c>
       <c r="M7" s="20"/>
-      <c r="N7" s="76">
+      <c r="N7" s="74">
         <f>N6/4</f>
         <v>43</v>
       </c>
@@ -1269,7 +1269,7 @@
       <c r="K8" s="20"/>
       <c r="L8" s="20"/>
       <c r="M8" s="20"/>
-      <c r="N8" s="76">
+      <c r="N8" s="74">
         <f>N7/6</f>
         <v>7.166666666666667</v>
       </c>
@@ -1297,7 +1297,7 @@
       <c r="K9" s="20"/>
       <c r="L9" s="20"/>
       <c r="M9" s="20"/>
-      <c r="N9" s="76">
+      <c r="N9" s="74">
         <f>97*N8/60</f>
         <v>11.586111111111112</v>
       </c>
@@ -1490,10 +1490,10 @@
     </row>
     <row r="19" spans="1:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="9"/>
-      <c r="B19" s="71" t="s">
+      <c r="B19" s="75" t="s">
         <v>11</v>
       </c>
-      <c r="C19" s="72"/>
+      <c r="C19" s="76"/>
       <c r="D19" s="17">
         <f>SUM(D10:D18)</f>
         <v>9467.8750664956679</v>

</xml_diff>

<commit_message>
Updated sensitivity analysis naar meest recente AzorModel
</commit_message>
<xml_diff>
--- a/Azores_Flight_Data_v4.xlsx
+++ b/Azores_Flight_Data_v4.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nils de Krom\Documents\GitHub\Operations_optimization_assignment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1262491-1440-4A01-81AE-D55E08F88EA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F763B94D-F469-49EB-A05A-58511A2923F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,12 +37,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="74">
   <si>
     <t>Cost per passenger</t>
-  </si>
-  <si>
-    <t>Destination</t>
   </si>
   <si>
     <t>Corvo</t>
@@ -961,7 +958,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:S1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
@@ -979,38 +976,38 @@
     <row r="1" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="47"/>
       <c r="B1" s="68" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C1" s="47"/>
       <c r="D1" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="G1" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="H1" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="I1" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="J1" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="K1" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="L1" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="E1" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="F1" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="G1" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="H1" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="I1" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="J1" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="K1" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="L1" s="9" t="s">
+      <c r="M1" s="75" t="s">
         <v>10</v>
-      </c>
-      <c r="M1" s="75" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -1018,46 +1015,46 @@
       <c r="B2" s="47"/>
       <c r="C2" s="47"/>
       <c r="D2" s="25" t="s">
+        <v>18</v>
+      </c>
+      <c r="E2" s="25" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" s="25" t="s">
+        <v>12</v>
+      </c>
+      <c r="G2" s="25" t="s">
+        <v>13</v>
+      </c>
+      <c r="H2" s="25" t="s">
+        <v>14</v>
+      </c>
+      <c r="I2" s="25" t="s">
+        <v>15</v>
+      </c>
+      <c r="J2" s="25" t="s">
+        <v>16</v>
+      </c>
+      <c r="K2" s="25" t="s">
+        <v>17</v>
+      </c>
+      <c r="L2" s="25" t="s">
         <v>19</v>
-      </c>
-      <c r="E2" s="25" t="s">
-        <v>12</v>
-      </c>
-      <c r="F2" s="25" t="s">
-        <v>13</v>
-      </c>
-      <c r="G2" s="25" t="s">
-        <v>14</v>
-      </c>
-      <c r="H2" s="25" t="s">
-        <v>15</v>
-      </c>
-      <c r="I2" s="25" t="s">
-        <v>16</v>
-      </c>
-      <c r="J2" s="25" t="s">
-        <v>17</v>
-      </c>
-      <c r="K2" s="25" t="s">
-        <v>18</v>
-      </c>
-      <c r="L2" s="25" t="s">
-        <v>20</v>
       </c>
       <c r="M2" s="76"/>
     </row>
     <row r="3" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="26" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C3" s="25" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D3" s="27">
-        <v>9307.8750664956679</v>
+        <v>28</v>
       </c>
       <c r="E3" s="28">
         <v>32</v>
@@ -1085,7 +1082,7 @@
       </c>
       <c r="M3" s="17">
         <f>SUM(D3:L3)</f>
-        <v>9568.8750664956679</v>
+        <v>289</v>
       </c>
     </row>
     <row r="4" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -1121,7 +1118,10 @@
       <c r="Q4" s="50"/>
     </row>
     <row r="5" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D5" s="71"/>
+      <c r="D5" s="71">
+        <f>D4/80</f>
+        <v>116.35</v>
+      </c>
       <c r="E5" s="71">
         <f>E4/80</f>
         <v>0.4</v>
@@ -1161,7 +1161,10 @@
       <c r="Q5" s="50"/>
     </row>
     <row r="6" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D6" s="71"/>
+      <c r="D6" s="71">
+        <f>ROUNDDOWN(D5,0)</f>
+        <v>116</v>
+      </c>
       <c r="E6" s="72">
         <f>ROUNDDOWN(E5,0)</f>
         <v>0</v>
@@ -1200,7 +1203,7 @@
         <v>172</v>
       </c>
       <c r="O6" s="73" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="P6" s="50"/>
       <c r="Q6" s="50"/>
@@ -1209,8 +1212,9 @@
       <c r="A7" s="47"/>
       <c r="B7" s="47"/>
       <c r="C7" s="47"/>
-      <c r="D7" s="26" t="s">
-        <v>1</v>
+      <c r="D7" s="1">
+        <f>D4-80*D6</f>
+        <v>28</v>
       </c>
       <c r="E7" s="20">
         <f>E4-80*E6</f>
@@ -1250,7 +1254,7 @@
         <v>43</v>
       </c>
       <c r="O7" s="52" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="P7" s="50"/>
       <c r="Q7" s="50"/>
@@ -1260,7 +1264,7 @@
       <c r="B8" s="68"/>
       <c r="C8" s="47"/>
       <c r="D8" s="25" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G8" s="20"/>
       <c r="H8" s="20"/>
@@ -1274,7 +1278,7 @@
         <v>7.166666666666667</v>
       </c>
       <c r="O8" s="53" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="P8" s="50"/>
       <c r="Q8" s="50"/>
@@ -1283,11 +1287,11 @@
     <row r="9" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="47"/>
       <c r="B9" s="68" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C9" s="47"/>
       <c r="D9" s="6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F9" s="20"/>
       <c r="G9" s="20"/>
@@ -1302,7 +1306,7 @@
         <v>11.586111111111112</v>
       </c>
       <c r="O9" s="53" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="P9" s="50"/>
       <c r="Q9" s="50"/>
@@ -1310,13 +1314,13 @@
     </row>
     <row r="10" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="48" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C10" s="25" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D10" s="29">
         <v>9307.8750664956679</v>
@@ -1338,10 +1342,10 @@
     <row r="11" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="47"/>
       <c r="B11" s="9" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C11" s="25" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D11" s="30">
         <v>20</v>
@@ -1363,10 +1367,10 @@
     <row r="12" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="47"/>
       <c r="B12" s="9" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C12" s="25" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D12" s="30">
         <v>20</v>
@@ -1388,10 +1392,10 @@
     <row r="13" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="47"/>
       <c r="B13" s="9" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C13" s="25" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D13" s="30">
         <v>20</v>
@@ -1413,10 +1417,10 @@
     <row r="14" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="47"/>
       <c r="B14" s="9" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C14" s="25" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D14" s="30">
         <v>20</v>
@@ -1429,10 +1433,10 @@
     <row r="15" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="47"/>
       <c r="B15" s="9" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C15" s="25" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D15" s="30">
         <v>20</v>
@@ -1445,10 +1449,10 @@
     <row r="16" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="47"/>
       <c r="B16" s="9" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C16" s="25" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D16" s="30">
         <v>20</v>
@@ -1461,10 +1465,10 @@
     <row r="17" spans="1:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="47"/>
       <c r="B17" s="9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C17" s="25" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D17" s="30">
         <v>20</v>
@@ -1476,10 +1480,10 @@
     <row r="18" spans="1:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="47"/>
       <c r="B18" s="9" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C18" s="25" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D18" s="30">
         <v>20</v>
@@ -1491,7 +1495,7 @@
     <row r="19" spans="1:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="9"/>
       <c r="B19" s="75" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C19" s="76"/>
       <c r="D19" s="17">
@@ -2578,39 +2582,39 @@
   <sheetData>
     <row r="1" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="67" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B1" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="D1" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="E1" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="F1" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="9" t="s">
+      <c r="G1" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="9" t="s">
+      <c r="H1" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="H1" s="9" t="s">
+      <c r="I1" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="I1" s="9" t="s">
+      <c r="J1" s="9" t="s">
         <v>9</v>
-      </c>
-      <c r="J1" s="9" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="9" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B2" s="31">
         <v>0</v>
@@ -2642,7 +2646,7 @@
     </row>
     <row r="3" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="9" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B3" s="19">
         <v>24</v>
@@ -2674,7 +2678,7 @@
     </row>
     <row r="4" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="9" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B4" s="19">
         <v>243</v>
@@ -2706,7 +2710,7 @@
     </row>
     <row r="5" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="9" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B5" s="19">
         <v>262</v>
@@ -2738,7 +2742,7 @@
     </row>
     <row r="6" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="9" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B6" s="19">
         <v>277</v>
@@ -2770,7 +2774,7 @@
     </row>
     <row r="7" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="9" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B7" s="19">
         <v>273</v>
@@ -2802,7 +2806,7 @@
     </row>
     <row r="8" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B8" s="19">
         <v>362</v>
@@ -2834,7 +2838,7 @@
     </row>
     <row r="9" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="9" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B9" s="19">
         <v>515</v>
@@ -2866,7 +2870,7 @@
     </row>
     <row r="10" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="9" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B10" s="22">
         <v>599</v>
@@ -2900,7 +2904,7 @@
     <row r="12" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="13" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="11" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="14" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3966,36 +3970,36 @@
   <sheetData>
     <row r="1" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" s="35" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="35" t="s">
-        <v>25</v>
-      </c>
       <c r="C1" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="36" t="s">
         <v>49</v>
-      </c>
-      <c r="G1" s="36" t="s">
-        <v>50</v>
       </c>
       <c r="H1" s="36" t="s">
         <v>0</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A2" s="57" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B2" s="58">
         <v>37</v>
@@ -4026,7 +4030,7 @@
     </row>
     <row r="3" spans="1:9" s="70" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A3" s="57" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B3" s="58">
         <v>37</v>
@@ -4057,7 +4061,7 @@
     </row>
     <row r="4" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A4" s="57" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B4" s="58">
         <v>80</v>
@@ -4088,7 +4092,7 @@
     </row>
     <row r="5" spans="1:9" s="70" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A5" s="57" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B5" s="58">
         <v>80</v>
@@ -4119,7 +4123,7 @@
     </row>
     <row r="6" spans="1:9" s="70" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A6" s="57" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B6" s="58">
         <v>80</v>
@@ -4150,7 +4154,7 @@
     </row>
     <row r="7" spans="1:9" s="70" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A7" s="57" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B7" s="58">
         <v>80</v>
@@ -4181,7 +4185,7 @@
     </row>
     <row r="8" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A8" s="57" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B8" s="58">
         <v>165</v>
@@ -4212,7 +4216,7 @@
     </row>
     <row r="9" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A9" s="57" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B9" s="58">
         <v>180</v>
@@ -4241,12 +4245,12 @@
         <v>9.1080000000000005</v>
       </c>
       <c r="I9" s="10" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A10" s="65" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B10" s="58">
         <v>186</v>
@@ -4275,12 +4279,12 @@
         <v>9.1080000000000005</v>
       </c>
       <c r="I10" s="10" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A11" s="57" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B11" s="58">
         <v>186</v>
@@ -4309,12 +4313,12 @@
         <v>9.1080000000000005</v>
       </c>
       <c r="I11" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A12" s="65" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B12" s="65">
         <v>190</v>
@@ -4343,20 +4347,20 @@
         <v>9.1080000000000005</v>
       </c>
       <c r="I12" s="37" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="15" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A15" s="38" t="s">
+        <v>53</v>
+      </c>
+      <c r="B15" s="39" t="s">
         <v>54</v>
-      </c>
-      <c r="B15" s="39" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="16" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A16" s="40" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B16" s="41">
         <v>3.32</v>
@@ -4364,7 +4368,7 @@
     </row>
     <row r="17" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A17" s="40" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B17" s="41">
         <v>4.05</v>
@@ -4372,7 +4376,7 @@
     </row>
     <row r="18" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A18" s="42" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B18" s="43">
         <v>4.7699999999999996</v>
@@ -4380,7 +4384,7 @@
     </row>
     <row r="21" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A21" s="36" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B21" s="1">
         <v>1.58</v>
@@ -4388,12 +4392,12 @@
     </row>
     <row r="23" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A23" s="36" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B24" s="1">
         <v>47.39</v>
@@ -4404,12 +4408,12 @@
         <v>0</v>
       </c>
       <c r="B27" s="44" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="28" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A28" s="41" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B28" s="1">
         <v>6.98</v>
@@ -4417,7 +4421,7 @@
     </row>
     <row r="29" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A29" s="41" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B29" s="1">
         <v>0.188</v>
@@ -4425,7 +4429,7 @@
     </row>
     <row r="30" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A30" s="41" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B30" s="1">
         <v>1.94</v>
@@ -4433,7 +4437,7 @@
     </row>
     <row r="31" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A31" s="45" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B31" s="46">
         <f>SUM(B28:B30)</f>
@@ -4470,48 +4474,48 @@
   <sheetData>
     <row r="1" spans="1:13" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="C1" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="D1" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="E1" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="F1" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="F1" s="7" t="s">
+      <c r="G1" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="G1" s="7" t="s">
+      <c r="H1" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="H1" s="8" t="s">
+      <c r="I1" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="I1" s="8" t="s">
-        <v>32</v>
-      </c>
       <c r="J1" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="K1" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="K1" s="11" t="s">
+      <c r="L1" s="62" t="s">
         <v>42</v>
       </c>
-      <c r="L1" s="62" t="s">
-        <v>43</v>
-      </c>
       <c r="M1" s="8" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="2" spans="1:13" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A2" s="57" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B2" s="58">
         <v>37</v>
@@ -4557,7 +4561,7 @@
     </row>
     <row r="3" spans="1:13" s="70" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A3" s="57" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B3" s="58">
         <v>37</v>
@@ -4603,7 +4607,7 @@
     </row>
     <row r="4" spans="1:13" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A4" s="57" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B4" s="58">
         <v>80</v>
@@ -4649,7 +4653,7 @@
     </row>
     <row r="5" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="57" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B5" s="58">
         <v>80</v>
@@ -4695,7 +4699,7 @@
     </row>
     <row r="6" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="57" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B6" s="58">
         <v>80</v>
@@ -4741,7 +4745,7 @@
     </row>
     <row r="7" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="57" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B7" s="58">
         <v>80</v>
@@ -4787,7 +4791,7 @@
     </row>
     <row r="11" spans="1:13" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="12" spans="1:13" ht="14.4" x14ac:dyDescent="0.3">
@@ -4795,10 +4799,10 @@
         <v>0.58899999999999997</v>
       </c>
       <c r="B12" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C12" s="3" t="s">
         <v>22</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>23</v>
       </c>
       <c r="D12" s="4">
         <f>0.88*A12</f>

</xml_diff>